<commit_message>
finished table extraction, starting fulltext extraction
</commit_message>
<xml_diff>
--- a/outputs/benchmark_combined.xlsx
+++ b/outputs/benchmark_combined.xlsx
@@ -3,28 +3,39 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Success Rate" sheetId="1" state="visible" r:id="rId1"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="PMC6449948_mean" sheetId="2" state="visible" r:id="rId2"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="PMC6449948_freq" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="PMC7767363_mean" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="PMC7767363_freq" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="PMC9322224_mean" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="PMC9322224_freq" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="PMC8536644_mean" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="PMC8536644_freq" sheetId="9" state="visible" r:id="rId9"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <b val="1"/>
+      <sz val="11"/>
     </font>
     <font>
       <b val="1"/>
@@ -38,12 +49,27 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -56,9 +82,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -428,11 +457,11 @@
   </sheetPr>
   <dimension ref="A1:A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -453,62 +482,62 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" s="2" t="inlineStr">
         <is>
           <t>Animal Model</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" s="2" t="inlineStr">
         <is>
           <t>Sample Size</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" s="2" t="inlineStr">
         <is>
           <t>Treatment 1</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="D1" s="2" t="inlineStr">
         <is>
           <t>Dose 1</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="E1" s="2" t="inlineStr">
         <is>
           <t>Units 1</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="F1" s="2" t="inlineStr">
         <is>
           <t>Treatment 2</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="G1" s="2" t="inlineStr">
         <is>
           <t>Dose 2</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="H1" s="2" t="inlineStr">
         <is>
           <t>Units 2</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="I1" s="2" t="inlineStr">
         <is>
           <t>Biomarker</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="J1" s="2" t="inlineStr">
         <is>
           <t>Value</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="K1" s="2" t="inlineStr">
         <is>
           <t>Units</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="L1" s="2" t="inlineStr">
         <is>
           <t>Variation</t>
         </is>
@@ -2139,7 +2168,7 @@
       <c r="H33" t="inlineStr"/>
       <c r="I33" t="inlineStr">
         <is>
-          <t>AST</t>
+          <t>Aspartate Transaminase (AST)</t>
         </is>
       </c>
       <c r="J33" t="inlineStr">
@@ -2177,7 +2206,7 @@
       <c r="H34" t="inlineStr"/>
       <c r="I34" t="inlineStr">
         <is>
-          <t>ALT</t>
+          <t>Alanine Transaminase (ALT)</t>
         </is>
       </c>
       <c r="J34" t="inlineStr">
@@ -2253,7 +2282,7 @@
       <c r="H36" t="inlineStr"/>
       <c r="I36" t="inlineStr">
         <is>
-          <t>AST</t>
+          <t>Aspartate Transaminase (AST)</t>
         </is>
       </c>
       <c r="J36" t="inlineStr">
@@ -2291,7 +2320,7 @@
       <c r="H37" t="inlineStr"/>
       <c r="I37" t="inlineStr">
         <is>
-          <t>ALT</t>
+          <t>Alanine Transaminase (ALT)</t>
         </is>
       </c>
       <c r="J37" t="inlineStr">
@@ -2391,7 +2420,7 @@
       <c r="H39" t="inlineStr"/>
       <c r="I39" t="inlineStr">
         <is>
-          <t>AST</t>
+          <t>Aspartate Transaminase (AST)</t>
         </is>
       </c>
       <c r="J39" t="inlineStr">
@@ -2441,7 +2470,7 @@
       <c r="H40" t="inlineStr"/>
       <c r="I40" t="inlineStr">
         <is>
-          <t>ALT</t>
+          <t>Alanine Transaminase (ALT)</t>
         </is>
       </c>
       <c r="J40" t="inlineStr">
@@ -2541,7 +2570,7 @@
       <c r="H42" t="inlineStr"/>
       <c r="I42" t="inlineStr">
         <is>
-          <t>AST</t>
+          <t>Aspartate Transaminase (AST)</t>
         </is>
       </c>
       <c r="J42" t="inlineStr">
@@ -2591,7 +2620,7 @@
       <c r="H43" t="inlineStr"/>
       <c r="I43" t="inlineStr">
         <is>
-          <t>ALT</t>
+          <t>Alanine Transaminase (ALT)</t>
         </is>
       </c>
       <c r="J43" t="inlineStr">
@@ -2691,7 +2720,7 @@
       <c r="H45" t="inlineStr"/>
       <c r="I45" t="inlineStr">
         <is>
-          <t>AST</t>
+          <t>Aspartate Transaminase (AST)</t>
         </is>
       </c>
       <c r="J45" t="inlineStr">
@@ -2741,7 +2770,7 @@
       <c r="H46" t="inlineStr"/>
       <c r="I46" t="inlineStr">
         <is>
-          <t>ALT</t>
+          <t>Alanine Transaminase (ALT)</t>
         </is>
       </c>
       <c r="J46" t="inlineStr">
@@ -2841,7 +2870,7 @@
       <c r="H48" t="inlineStr"/>
       <c r="I48" t="inlineStr">
         <is>
-          <t>AST</t>
+          <t>Aspartate Transaminase (AST)</t>
         </is>
       </c>
       <c r="J48" t="inlineStr">
@@ -2891,7 +2920,7 @@
       <c r="H49" t="inlineStr"/>
       <c r="I49" t="inlineStr">
         <is>
-          <t>ALT</t>
+          <t>Alanine Transaminase (ALT)</t>
         </is>
       </c>
       <c r="J49" t="inlineStr">
@@ -2991,7 +3020,7 @@
       <c r="H51" t="inlineStr"/>
       <c r="I51" t="inlineStr">
         <is>
-          <t>AST</t>
+          <t>Aspartate Transaminase (AST)</t>
         </is>
       </c>
       <c r="J51" t="inlineStr">
@@ -3041,7 +3070,7 @@
       <c r="H52" t="inlineStr"/>
       <c r="I52" t="inlineStr">
         <is>
-          <t>ALT</t>
+          <t>Alanine Transaminase (ALT)</t>
         </is>
       </c>
       <c r="J52" t="inlineStr">
@@ -3141,7 +3170,7 @@
       <c r="H54" t="inlineStr"/>
       <c r="I54" t="inlineStr">
         <is>
-          <t>AST</t>
+          <t>Aspartate Transaminase (AST)</t>
         </is>
       </c>
       <c r="J54" t="inlineStr">
@@ -3191,7 +3220,7 @@
       <c r="H55" t="inlineStr"/>
       <c r="I55" t="inlineStr">
         <is>
-          <t>ALT</t>
+          <t>Alanine Transaminase (ALT)</t>
         </is>
       </c>
       <c r="J55" t="inlineStr">
@@ -3291,7 +3320,7 @@
       <c r="H57" t="inlineStr"/>
       <c r="I57" t="inlineStr">
         <is>
-          <t>AST</t>
+          <t>Aspartate Transaminase (AST)</t>
         </is>
       </c>
       <c r="J57" t="inlineStr">
@@ -3341,7 +3370,7 @@
       <c r="H58" t="inlineStr"/>
       <c r="I58" t="inlineStr">
         <is>
-          <t>ALT</t>
+          <t>Alanine Transaminase (ALT)</t>
         </is>
       </c>
       <c r="J58" t="inlineStr">
@@ -3441,7 +3470,7 @@
       <c r="H60" t="inlineStr"/>
       <c r="I60" t="inlineStr">
         <is>
-          <t>AST</t>
+          <t>Aspartate Transaminase (AST)</t>
         </is>
       </c>
       <c r="J60" t="inlineStr">
@@ -3491,7 +3520,7 @@
       <c r="H61" t="inlineStr"/>
       <c r="I61" t="inlineStr">
         <is>
-          <t>ALT</t>
+          <t>Alanine Transaminase (ALT)</t>
         </is>
       </c>
       <c r="J61" t="inlineStr">
@@ -3591,7 +3620,7 @@
       <c r="H63" t="inlineStr"/>
       <c r="I63" t="inlineStr">
         <is>
-          <t>AST</t>
+          <t>Aspartate Transaminase (AST)</t>
         </is>
       </c>
       <c r="J63" t="inlineStr">
@@ -3641,7 +3670,7 @@
       <c r="H64" t="inlineStr"/>
       <c r="I64" t="inlineStr">
         <is>
-          <t>ALT</t>
+          <t>Alanine Transaminase (ALT)</t>
         </is>
       </c>
       <c r="J64" t="inlineStr">
@@ -3765,7 +3794,7 @@
       </c>
       <c r="I66" t="inlineStr">
         <is>
-          <t>AST</t>
+          <t>Aspartate Transaminase (AST)</t>
         </is>
       </c>
       <c r="J66" t="inlineStr">
@@ -3827,7 +3856,7 @@
       </c>
       <c r="I67" t="inlineStr">
         <is>
-          <t>ALT</t>
+          <t>Alanine Transaminase (ALT)</t>
         </is>
       </c>
       <c r="J67" t="inlineStr">
@@ -3951,7 +3980,7 @@
       </c>
       <c r="I69" t="inlineStr">
         <is>
-          <t>AST</t>
+          <t>Aspartate Transaminase (AST)</t>
         </is>
       </c>
       <c r="J69" t="inlineStr">
@@ -4013,7 +4042,7 @@
       </c>
       <c r="I70" t="inlineStr">
         <is>
-          <t>ALT</t>
+          <t>Alanine Transaminase (ALT)</t>
         </is>
       </c>
       <c r="J70" t="inlineStr">
@@ -4137,7 +4166,7 @@
       </c>
       <c r="I72" t="inlineStr">
         <is>
-          <t>AST</t>
+          <t>Aspartate Transaminase (AST)</t>
         </is>
       </c>
       <c r="J72" t="inlineStr">
@@ -4199,7 +4228,7 @@
       </c>
       <c r="I73" t="inlineStr">
         <is>
-          <t>ALT</t>
+          <t>Alanine Transaminase (ALT)</t>
         </is>
       </c>
       <c r="J73" t="inlineStr">
@@ -4323,7 +4352,7 @@
       </c>
       <c r="I75" t="inlineStr">
         <is>
-          <t>AST</t>
+          <t>Aspartate Transaminase (AST)</t>
         </is>
       </c>
       <c r="J75" t="inlineStr">
@@ -4385,7 +4414,7 @@
       </c>
       <c r="I76" t="inlineStr">
         <is>
-          <t>ALT</t>
+          <t>Alanine Transaminase (ALT)</t>
         </is>
       </c>
       <c r="J76" t="inlineStr">
@@ -4424,57 +4453,57 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" s="2" t="inlineStr">
         <is>
           <t>Animal Model</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" s="2" t="inlineStr">
         <is>
           <t>Sample Size</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" s="2" t="inlineStr">
         <is>
           <t>Treatment 1</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="D1" s="2" t="inlineStr">
         <is>
           <t>Dose 1</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="E1" s="2" t="inlineStr">
         <is>
           <t>Units 1</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="F1" s="2" t="inlineStr">
         <is>
           <t>Treatment 2</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="G1" s="2" t="inlineStr">
         <is>
           <t>Dose 2</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="H1" s="2" t="inlineStr">
         <is>
           <t>Units 2</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="I1" s="2" t="inlineStr">
         <is>
           <t>Biomarker</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="J1" s="2" t="inlineStr">
         <is>
           <t>Frequency</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="K1" s="2" t="inlineStr">
         <is>
           <t>Severity</t>
         </is>
@@ -4909,4 +4938,4082 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:L34"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Animal Model</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Sample Size</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Treatment 1</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Dose 1</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Units 1</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Treatment 2</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Dose 2</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Units 2</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Biomarker</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Value</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Units</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Variation</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>mouse</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>Platelet count</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>697.50</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>10/muL</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>64.16</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>mouse</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>Platelet</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>697.50</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>10/muL</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>64.16</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>mouse</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>Red blood cells</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>8.38</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>M/muL</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>0.27</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>mouse</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>Hematocrit</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>45.86</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>%</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>2.37</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>mouse</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>Neutrophil count</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>0.54</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>10/muL</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>0.09</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>mouse</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>Lymphocyte count</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>2.22</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>10/muL</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>0.50</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>mouse</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>ALT</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>26.28</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>U/L</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>6.33</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>mouse</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>AST</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>89.46</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>U/L</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>17.86</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>mouse</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>ALP</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>295.11</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>U/L</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>99.65</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>mouse</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>GGT</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>4.97</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>U/L</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>1.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>mouse</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>Total bilirubin</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>0.06</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>U/L</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>0.03</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>mouse</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>DM1</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>60</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>μg/kg</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>Platelet count</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>632.40</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>10/muL</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>101.64</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>mouse</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>DM1</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>60</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>μg/kg</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>Platelet</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>632.40</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>10/muL</t>
+        </is>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>101.64</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>mouse</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>DM1</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>60</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>μg/kg</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>Red blood cells</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>8.08</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>M/muL</t>
+        </is>
+      </c>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>0.35</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>mouse</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>DM1</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>60</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>μg/kg</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>Hematocrit</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>46.38</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>%</t>
+        </is>
+      </c>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>1.41</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>mouse</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>DM1</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>60</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>μg/kg</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>Neutrophil count</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>0.37</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>10/muL</t>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>0.15</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>mouse</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>DM1</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>60</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>μg/kg</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>Lymphocyte count</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>1.78</t>
+        </is>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>10/muL</t>
+        </is>
+      </c>
+      <c r="L18" t="inlineStr">
+        <is>
+          <t>0.89</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>mouse</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>DM1</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>60</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>μg/kg</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>ALT</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>32.29</t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>U/L</t>
+        </is>
+      </c>
+      <c r="L19" t="inlineStr">
+        <is>
+          <t>14.33</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>mouse</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>DM1</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>60</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>μg/kg</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>AST</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>89.20</t>
+        </is>
+      </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>U/L</t>
+        </is>
+      </c>
+      <c r="L20" t="inlineStr">
+        <is>
+          <t>11.66</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>mouse</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>DM1</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>60</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>μg/kg</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>ALP</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>292.01</t>
+        </is>
+      </c>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>U/L</t>
+        </is>
+      </c>
+      <c r="L21" t="inlineStr">
+        <is>
+          <t>84.44</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>mouse</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>DM1</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>60</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>μg/kg</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>GGT</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>7.02</t>
+        </is>
+      </c>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>U/L</t>
+        </is>
+      </c>
+      <c r="L22" t="inlineStr">
+        <is>
+          <t>2.11</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>mouse</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>DM1</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>60</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>μg/kg</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>Total bilirubin</t>
+        </is>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>0.07</t>
+        </is>
+      </c>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>U/L</t>
+        </is>
+      </c>
+      <c r="L23" t="inlineStr">
+        <is>
+          <t>0.03</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>mouse</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>ApDC</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>2.7</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>mg/kg</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>Platelet count</t>
+        </is>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>425.33</t>
+        </is>
+      </c>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>10/muL</t>
+        </is>
+      </c>
+      <c r="L24" t="inlineStr">
+        <is>
+          <t>66.11</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>mouse</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>ApDC</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>2.7</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>mg/kg</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>Platelet</t>
+        </is>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>425.33</t>
+        </is>
+      </c>
+      <c r="K25" t="inlineStr">
+        <is>
+          <t>10/muL</t>
+        </is>
+      </c>
+      <c r="L25" t="inlineStr">
+        <is>
+          <t>66.11</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>mouse</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>ApDC</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>2.7</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>mg/kg</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>Red blood cells</t>
+        </is>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>7.69</t>
+        </is>
+      </c>
+      <c r="K26" t="inlineStr">
+        <is>
+          <t>M/muL</t>
+        </is>
+      </c>
+      <c r="L26" t="inlineStr">
+        <is>
+          <t>0.34</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>mouse</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>ApDC</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>2.7</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>mg/kg</t>
+        </is>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>Hematocrit</t>
+        </is>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>43.17</t>
+        </is>
+      </c>
+      <c r="K27" t="inlineStr">
+        <is>
+          <t>%</t>
+        </is>
+      </c>
+      <c r="L27" t="inlineStr">
+        <is>
+          <t>1.20</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>mouse</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>ApDC</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>2.7</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>mg/kg</t>
+        </is>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>Neutrophil count</t>
+        </is>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>0.31</t>
+        </is>
+      </c>
+      <c r="K28" t="inlineStr">
+        <is>
+          <t>10/muL</t>
+        </is>
+      </c>
+      <c r="L28" t="inlineStr">
+        <is>
+          <t>0.11</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>mouse</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>ApDC</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>2.7</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>mg/kg</t>
+        </is>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>Lymphocyte count</t>
+        </is>
+      </c>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>1.55</t>
+        </is>
+      </c>
+      <c r="K29" t="inlineStr">
+        <is>
+          <t>10/muL</t>
+        </is>
+      </c>
+      <c r="L29" t="inlineStr">
+        <is>
+          <t>0.18</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>mouse</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>ApDC</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>2.7</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>mg/kg</t>
+        </is>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>ALT</t>
+        </is>
+      </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>42.93</t>
+        </is>
+      </c>
+      <c r="K30" t="inlineStr">
+        <is>
+          <t>U/L</t>
+        </is>
+      </c>
+      <c r="L30" t="inlineStr">
+        <is>
+          <t>14.86</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>mouse</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>ApDC</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>2.7</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>mg/kg</t>
+        </is>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>AST</t>
+        </is>
+      </c>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>95.35</t>
+        </is>
+      </c>
+      <c r="K31" t="inlineStr">
+        <is>
+          <t>U/L</t>
+        </is>
+      </c>
+      <c r="L31" t="inlineStr">
+        <is>
+          <t>20.89</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>mouse</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>ApDC</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>2.7</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>mg/kg</t>
+        </is>
+      </c>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>ALP</t>
+        </is>
+      </c>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t>211.76</t>
+        </is>
+      </c>
+      <c r="K32" t="inlineStr">
+        <is>
+          <t>U/L</t>
+        </is>
+      </c>
+      <c r="L32" t="inlineStr">
+        <is>
+          <t>44.13</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>mouse</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>ApDC</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>2.7</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>mg/kg</t>
+        </is>
+      </c>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>GGT</t>
+        </is>
+      </c>
+      <c r="J33" t="inlineStr">
+        <is>
+          <t>6.28</t>
+        </is>
+      </c>
+      <c r="K33" t="inlineStr">
+        <is>
+          <t>U/L</t>
+        </is>
+      </c>
+      <c r="L33" t="inlineStr">
+        <is>
+          <t>3.67</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>mouse</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>ApDC</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>2.7</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>mg/kg</t>
+        </is>
+      </c>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>Total bilirubin</t>
+        </is>
+      </c>
+      <c r="J34" t="inlineStr">
+        <is>
+          <t>0.07</t>
+        </is>
+      </c>
+      <c r="K34" t="inlineStr">
+        <is>
+          <t>U/L</t>
+        </is>
+      </c>
+      <c r="L34" t="inlineStr">
+        <is>
+          <t>0.02</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:L76"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>Animal Model</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>Sample Size</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>Treatment 1</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>Dose 1</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
+          <t>Units 1</t>
+        </is>
+      </c>
+      <c r="F1" s="2" t="inlineStr">
+        <is>
+          <t>Treatment 2</t>
+        </is>
+      </c>
+      <c r="G1" s="2" t="inlineStr">
+        <is>
+          <t>Dose 2</t>
+        </is>
+      </c>
+      <c r="H1" s="2" t="inlineStr">
+        <is>
+          <t>Units 2</t>
+        </is>
+      </c>
+      <c r="I1" s="2" t="inlineStr">
+        <is>
+          <t>Biomarker</t>
+        </is>
+      </c>
+      <c r="J1" s="2" t="inlineStr">
+        <is>
+          <t>Value</t>
+        </is>
+      </c>
+      <c r="K1" s="2" t="inlineStr">
+        <is>
+          <t>Units</t>
+        </is>
+      </c>
+      <c r="L1" s="2" t="inlineStr">
+        <is>
+          <t>Variation</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>Body weight</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>21.26</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>g</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>1.24 *</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>Tumour weight</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>1.45</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>g</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>0.43</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>Inhibition rate</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>percent</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>methotrexate</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>0.2</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>mg/kg</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>Body weight</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>20.88</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>g</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>0.79 *</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>methotrexate</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>0.2</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>mg/kg</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>Tumour weight</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>1.21</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>g</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>0.41</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>methotrexate</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>0.2</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>mg/kg</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>Inhibition rate</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>16.55</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>percent</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>aspartame</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>40</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>mg/kg</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>Body weight</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>19.49</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>g</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>0.30 *</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>aspartame</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>40</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>mg/kg</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>Tumour weight</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>NG</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>g</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>aspartame</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>40</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>mg/kg</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>Inhibition rate</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>percent</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>Body weight</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>19.30</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>g</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>0.06 *</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>Tumour weight</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>NG</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>g</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>Inhibition rate</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>percent</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>Body weight</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>19.45</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>g</t>
+        </is>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>0.10 *</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>Tumour weight</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>NG</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>g</t>
+        </is>
+      </c>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>Inhibition rate</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>percent</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>Body weight</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>19.66</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>g</t>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>0.13 *</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>Tumour weight</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>NG</t>
+        </is>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>g</t>
+        </is>
+      </c>
+      <c r="L18" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>Inhibition rate</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>percent</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>Body weight</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>19.33</t>
+        </is>
+      </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>g</t>
+        </is>
+      </c>
+      <c r="L20" t="inlineStr">
+        <is>
+          <t>0.16 *</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>Tumour weight</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>NG</t>
+        </is>
+      </c>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>g</t>
+        </is>
+      </c>
+      <c r="L21" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>Inhibition rate</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>percent</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>Body weight</t>
+        </is>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>19.50</t>
+        </is>
+      </c>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>g</t>
+        </is>
+      </c>
+      <c r="L23" t="inlineStr">
+        <is>
+          <t>0.30 *</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>Tumour weight</t>
+        </is>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>NG</t>
+        </is>
+      </c>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>g</t>
+        </is>
+      </c>
+      <c r="L24" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>Inhibition rate</t>
+        </is>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="K25" t="inlineStr">
+        <is>
+          <t>percent</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>Body weight</t>
+        </is>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>21.00</t>
+        </is>
+      </c>
+      <c r="K26" t="inlineStr">
+        <is>
+          <t>g</t>
+        </is>
+      </c>
+      <c r="L26" t="inlineStr">
+        <is>
+          <t>0.40 *</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>Tumour weight</t>
+        </is>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>2.27</t>
+        </is>
+      </c>
+      <c r="K27" t="inlineStr">
+        <is>
+          <t>g</t>
+        </is>
+      </c>
+      <c r="L27" t="inlineStr">
+        <is>
+          <t>0.28</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>Inhibition rate</t>
+        </is>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>-56.55</t>
+        </is>
+      </c>
+      <c r="K28" t="inlineStr">
+        <is>
+          <t>percent</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>Body weight</t>
+        </is>
+      </c>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>20.59</t>
+        </is>
+      </c>
+      <c r="K29" t="inlineStr">
+        <is>
+          <t>g</t>
+        </is>
+      </c>
+      <c r="L29" t="inlineStr">
+        <is>
+          <t>0.36 *</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>Tumour weight</t>
+        </is>
+      </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>3.64</t>
+        </is>
+      </c>
+      <c r="K30" t="inlineStr">
+        <is>
+          <t>g</t>
+        </is>
+      </c>
+      <c r="L30" t="inlineStr">
+        <is>
+          <t>0.23</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>Inhibition rate</t>
+        </is>
+      </c>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>-151.03</t>
+        </is>
+      </c>
+      <c r="K31" t="inlineStr">
+        <is>
+          <t>percent</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>rat</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>Total Bilirubin</t>
+        </is>
+      </c>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t>3.43</t>
+        </is>
+      </c>
+      <c r="K32" t="inlineStr">
+        <is>
+          <t>mg/dl</t>
+        </is>
+      </c>
+      <c r="L32" t="inlineStr">
+        <is>
+          <t>0.40</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>rat</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>AST</t>
+        </is>
+      </c>
+      <c r="J33" t="inlineStr">
+        <is>
+          <t>120.67</t>
+        </is>
+      </c>
+      <c r="K33" t="inlineStr">
+        <is>
+          <t>U/l</t>
+        </is>
+      </c>
+      <c r="L33" t="inlineStr">
+        <is>
+          <t>1.53</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>rat</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>ALT</t>
+        </is>
+      </c>
+      <c r="J34" t="inlineStr">
+        <is>
+          <t>36.00</t>
+        </is>
+      </c>
+      <c r="K34" t="inlineStr">
+        <is>
+          <t>U/l</t>
+        </is>
+      </c>
+      <c r="L34" t="inlineStr">
+        <is>
+          <t>2.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>rat</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>methotrexate</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>0.2</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>mg/kg</t>
+        </is>
+      </c>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>Total Bilirubin</t>
+        </is>
+      </c>
+      <c r="J35" t="inlineStr">
+        <is>
+          <t>2.13</t>
+        </is>
+      </c>
+      <c r="K35" t="inlineStr">
+        <is>
+          <t>mg/dl</t>
+        </is>
+      </c>
+      <c r="L35" t="inlineStr">
+        <is>
+          <t>0.95</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>rat</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>methotrexate</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>0.2</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>mg/kg</t>
+        </is>
+      </c>
+      <c r="I36" t="inlineStr">
+        <is>
+          <t>AST</t>
+        </is>
+      </c>
+      <c r="J36" t="inlineStr">
+        <is>
+          <t>214.67</t>
+        </is>
+      </c>
+      <c r="K36" t="inlineStr">
+        <is>
+          <t>U/l</t>
+        </is>
+      </c>
+      <c r="L36" t="inlineStr">
+        <is>
+          <t>1.53 *</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>rat</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>methotrexate</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>0.2</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>mg/kg</t>
+        </is>
+      </c>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>ALT</t>
+        </is>
+      </c>
+      <c r="J37" t="inlineStr">
+        <is>
+          <t>53.67</t>
+        </is>
+      </c>
+      <c r="K37" t="inlineStr">
+        <is>
+          <t>U/l</t>
+        </is>
+      </c>
+      <c r="L37" t="inlineStr">
+        <is>
+          <t>1.53</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>rat</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>aspartame</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>40</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>mg/kg</t>
+        </is>
+      </c>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>Total Bilirubin</t>
+        </is>
+      </c>
+      <c r="J38" t="inlineStr">
+        <is>
+          <t>5.27</t>
+        </is>
+      </c>
+      <c r="K38" t="inlineStr">
+        <is>
+          <t>mg/dl</t>
+        </is>
+      </c>
+      <c r="L38" t="inlineStr">
+        <is>
+          <t>0.59</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>rat</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>aspartame</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>40</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>mg/kg</t>
+        </is>
+      </c>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>AST</t>
+        </is>
+      </c>
+      <c r="J39" t="inlineStr">
+        <is>
+          <t>265.00</t>
+        </is>
+      </c>
+      <c r="K39" t="inlineStr">
+        <is>
+          <t>U/l</t>
+        </is>
+      </c>
+      <c r="L39" t="inlineStr">
+        <is>
+          <t>2.00 *</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>rat</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>aspartame</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>40</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>mg/kg</t>
+        </is>
+      </c>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>ALT</t>
+        </is>
+      </c>
+      <c r="J40" t="inlineStr">
+        <is>
+          <t>95.67</t>
+        </is>
+      </c>
+      <c r="K40" t="inlineStr">
+        <is>
+          <t>U/l</t>
+        </is>
+      </c>
+      <c r="L40" t="inlineStr">
+        <is>
+          <t>1.53 *</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="I41" t="inlineStr">
+        <is>
+          <t>Total Bilirubin</t>
+        </is>
+      </c>
+      <c r="J41" t="inlineStr">
+        <is>
+          <t>4.43</t>
+        </is>
+      </c>
+      <c r="K41" t="inlineStr">
+        <is>
+          <t>mg/dl</t>
+        </is>
+      </c>
+      <c r="L41" t="inlineStr">
+        <is>
+          <t>0.40</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="I42" t="inlineStr">
+        <is>
+          <t>AST</t>
+        </is>
+      </c>
+      <c r="J42" t="inlineStr">
+        <is>
+          <t>153.33</t>
+        </is>
+      </c>
+      <c r="K42" t="inlineStr">
+        <is>
+          <t>U/l</t>
+        </is>
+      </c>
+      <c r="L42" t="inlineStr">
+        <is>
+          <t>1.53</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="I43" t="inlineStr">
+        <is>
+          <t>ALT</t>
+        </is>
+      </c>
+      <c r="J43" t="inlineStr">
+        <is>
+          <t>38.67</t>
+        </is>
+      </c>
+      <c r="K43" t="inlineStr">
+        <is>
+          <t>U/l</t>
+        </is>
+      </c>
+      <c r="L43" t="inlineStr">
+        <is>
+          <t>1.53</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="I44" t="inlineStr">
+        <is>
+          <t>Total Bilirubin</t>
+        </is>
+      </c>
+      <c r="J44" t="inlineStr">
+        <is>
+          <t>5.75</t>
+        </is>
+      </c>
+      <c r="K44" t="inlineStr">
+        <is>
+          <t>mg/dl</t>
+        </is>
+      </c>
+      <c r="L44" t="inlineStr">
+        <is>
+          <t>0.35</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="I45" t="inlineStr">
+        <is>
+          <t>AST</t>
+        </is>
+      </c>
+      <c r="J45" t="inlineStr">
+        <is>
+          <t>125.33</t>
+        </is>
+      </c>
+      <c r="K45" t="inlineStr">
+        <is>
+          <t>U/l</t>
+        </is>
+      </c>
+      <c r="L45" t="inlineStr">
+        <is>
+          <t>93.82</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="I46" t="inlineStr">
+        <is>
+          <t>ALT</t>
+        </is>
+      </c>
+      <c r="J46" t="inlineStr">
+        <is>
+          <t>41.67</t>
+        </is>
+      </c>
+      <c r="K46" t="inlineStr">
+        <is>
+          <t>U/l</t>
+        </is>
+      </c>
+      <c r="L46" t="inlineStr">
+        <is>
+          <t>1.53</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="I47" t="inlineStr">
+        <is>
+          <t>Total Bilirubin</t>
+        </is>
+      </c>
+      <c r="J47" t="inlineStr">
+        <is>
+          <t>4.87</t>
+        </is>
+      </c>
+      <c r="K47" t="inlineStr">
+        <is>
+          <t>mg/dl</t>
+        </is>
+      </c>
+      <c r="L47" t="inlineStr">
+        <is>
+          <t>0.35</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="I48" t="inlineStr">
+        <is>
+          <t>AST</t>
+        </is>
+      </c>
+      <c r="J48" t="inlineStr">
+        <is>
+          <t>105.00</t>
+        </is>
+      </c>
+      <c r="K48" t="inlineStr">
+        <is>
+          <t>U/l</t>
+        </is>
+      </c>
+      <c r="L48" t="inlineStr">
+        <is>
+          <t>1.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="I49" t="inlineStr">
+        <is>
+          <t>ALT</t>
+        </is>
+      </c>
+      <c r="J49" t="inlineStr">
+        <is>
+          <t>47.00</t>
+        </is>
+      </c>
+      <c r="K49" t="inlineStr">
+        <is>
+          <t>U/l</t>
+        </is>
+      </c>
+      <c r="L49" t="inlineStr">
+        <is>
+          <t>1.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="I50" t="inlineStr">
+        <is>
+          <t>Total Bilirubin</t>
+        </is>
+      </c>
+      <c r="J50" t="inlineStr">
+        <is>
+          <t>5.13</t>
+        </is>
+      </c>
+      <c r="K50" t="inlineStr">
+        <is>
+          <t>mg/dl</t>
+        </is>
+      </c>
+      <c r="L50" t="inlineStr">
+        <is>
+          <t>0.67</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="I51" t="inlineStr">
+        <is>
+          <t>AST</t>
+        </is>
+      </c>
+      <c r="J51" t="inlineStr">
+        <is>
+          <t>115.00</t>
+        </is>
+      </c>
+      <c r="K51" t="inlineStr">
+        <is>
+          <t>U/l</t>
+        </is>
+      </c>
+      <c r="L51" t="inlineStr">
+        <is>
+          <t>11.27</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="I52" t="inlineStr">
+        <is>
+          <t>ALT</t>
+        </is>
+      </c>
+      <c r="J52" t="inlineStr">
+        <is>
+          <t>52.67</t>
+        </is>
+      </c>
+      <c r="K52" t="inlineStr">
+        <is>
+          <t>U/l</t>
+        </is>
+      </c>
+      <c r="L52" t="inlineStr">
+        <is>
+          <t>2.51</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="I53" t="inlineStr">
+        <is>
+          <t>Total Bilirubin</t>
+        </is>
+      </c>
+      <c r="J53" t="inlineStr">
+        <is>
+          <t>4.47</t>
+        </is>
+      </c>
+      <c r="K53" t="inlineStr">
+        <is>
+          <t>mg/dl</t>
+        </is>
+      </c>
+      <c r="L53" t="inlineStr">
+        <is>
+          <t>0.35</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="I54" t="inlineStr">
+        <is>
+          <t>AST</t>
+        </is>
+      </c>
+      <c r="J54" t="inlineStr">
+        <is>
+          <t>98.67</t>
+        </is>
+      </c>
+      <c r="K54" t="inlineStr">
+        <is>
+          <t>U/l</t>
+        </is>
+      </c>
+      <c r="L54" t="inlineStr">
+        <is>
+          <t>1.53</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="I55" t="inlineStr">
+        <is>
+          <t>ALT</t>
+        </is>
+      </c>
+      <c r="J55" t="inlineStr">
+        <is>
+          <t>26.33</t>
+        </is>
+      </c>
+      <c r="K55" t="inlineStr">
+        <is>
+          <t>U/l</t>
+        </is>
+      </c>
+      <c r="L55" t="inlineStr">
+        <is>
+          <t>1.15</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="I56" t="inlineStr">
+        <is>
+          <t>Total Bilirubin</t>
+        </is>
+      </c>
+      <c r="J56" t="inlineStr">
+        <is>
+          <t>3.00</t>
+        </is>
+      </c>
+      <c r="K56" t="inlineStr">
+        <is>
+          <t>mg/dl</t>
+        </is>
+      </c>
+      <c r="L56" t="inlineStr">
+        <is>
+          <t>0.50</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="I57" t="inlineStr">
+        <is>
+          <t>AST</t>
+        </is>
+      </c>
+      <c r="J57" t="inlineStr">
+        <is>
+          <t>173.33</t>
+        </is>
+      </c>
+      <c r="K57" t="inlineStr">
+        <is>
+          <t>U/l</t>
+        </is>
+      </c>
+      <c r="L57" t="inlineStr">
+        <is>
+          <t>1.53</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="I58" t="inlineStr">
+        <is>
+          <t>ALT</t>
+        </is>
+      </c>
+      <c r="J58" t="inlineStr">
+        <is>
+          <t>57.00</t>
+        </is>
+      </c>
+      <c r="K58" t="inlineStr">
+        <is>
+          <t>U/l</t>
+        </is>
+      </c>
+      <c r="L58" t="inlineStr">
+        <is>
+          <t>1.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="I59" t="inlineStr">
+        <is>
+          <t>Total Bilirubin</t>
+        </is>
+      </c>
+      <c r="J59" t="inlineStr">
+        <is>
+          <t>2.87</t>
+        </is>
+      </c>
+      <c r="K59" t="inlineStr">
+        <is>
+          <t>mg/dl</t>
+        </is>
+      </c>
+      <c r="L59" t="inlineStr">
+        <is>
+          <t>0.35</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="I60" t="inlineStr">
+        <is>
+          <t>AST</t>
+        </is>
+      </c>
+      <c r="J60" t="inlineStr">
+        <is>
+          <t>121.00</t>
+        </is>
+      </c>
+      <c r="K60" t="inlineStr">
+        <is>
+          <t>U/l</t>
+        </is>
+      </c>
+      <c r="L60" t="inlineStr">
+        <is>
+          <t>2.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="I61" t="inlineStr">
+        <is>
+          <t>ALT</t>
+        </is>
+      </c>
+      <c r="J61" t="inlineStr">
+        <is>
+          <t>49.00</t>
+        </is>
+      </c>
+      <c r="K61" t="inlineStr">
+        <is>
+          <t>U/l</t>
+        </is>
+      </c>
+      <c r="L61" t="inlineStr">
+        <is>
+          <t>1.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="I62" t="inlineStr">
+        <is>
+          <t>Total Bilirubin</t>
+        </is>
+      </c>
+      <c r="J62" t="inlineStr">
+        <is>
+          <t>3.40</t>
+        </is>
+      </c>
+      <c r="K62" t="inlineStr">
+        <is>
+          <t>mg/dl</t>
+        </is>
+      </c>
+      <c r="L62" t="inlineStr">
+        <is>
+          <t>0.40</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="I63" t="inlineStr">
+        <is>
+          <t>AST</t>
+        </is>
+      </c>
+      <c r="J63" t="inlineStr">
+        <is>
+          <t>153.67</t>
+        </is>
+      </c>
+      <c r="K63" t="inlineStr">
+        <is>
+          <t>U/l</t>
+        </is>
+      </c>
+      <c r="L63" t="inlineStr">
+        <is>
+          <t>1.53</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="I64" t="inlineStr">
+        <is>
+          <t>ALT</t>
+        </is>
+      </c>
+      <c r="J64" t="inlineStr">
+        <is>
+          <t>49.33</t>
+        </is>
+      </c>
+      <c r="K64" t="inlineStr">
+        <is>
+          <t>U/l</t>
+        </is>
+      </c>
+      <c r="L64" t="inlineStr">
+        <is>
+          <t>0.58</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="I65" t="inlineStr">
+        <is>
+          <t>Total Bilirubin</t>
+        </is>
+      </c>
+      <c r="J65" t="inlineStr">
+        <is>
+          <t>2.77</t>
+        </is>
+      </c>
+      <c r="K65" t="inlineStr">
+        <is>
+          <t>mg/dl</t>
+        </is>
+      </c>
+      <c r="L65" t="inlineStr">
+        <is>
+          <t>0.45</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="I66" t="inlineStr">
+        <is>
+          <t>AST</t>
+        </is>
+      </c>
+      <c r="J66" t="inlineStr">
+        <is>
+          <t>166.67</t>
+        </is>
+      </c>
+      <c r="K66" t="inlineStr">
+        <is>
+          <t>U/l</t>
+        </is>
+      </c>
+      <c r="L66" t="inlineStr">
+        <is>
+          <t>56.62</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="I67" t="inlineStr">
+        <is>
+          <t>ALT</t>
+        </is>
+      </c>
+      <c r="J67" t="inlineStr">
+        <is>
+          <t>103.00</t>
+        </is>
+      </c>
+      <c r="K67" t="inlineStr">
+        <is>
+          <t>U/l</t>
+        </is>
+      </c>
+      <c r="L67" t="inlineStr">
+        <is>
+          <t>2.00 *</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="I68" t="inlineStr">
+        <is>
+          <t>Total Bilirubin</t>
+        </is>
+      </c>
+      <c r="J68" t="inlineStr">
+        <is>
+          <t>2.43</t>
+        </is>
+      </c>
+      <c r="K68" t="inlineStr">
+        <is>
+          <t>mg/dl</t>
+        </is>
+      </c>
+      <c r="L68" t="inlineStr">
+        <is>
+          <t>0.40</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="I69" t="inlineStr">
+        <is>
+          <t>AST</t>
+        </is>
+      </c>
+      <c r="J69" t="inlineStr">
+        <is>
+          <t>108.00</t>
+        </is>
+      </c>
+      <c r="K69" t="inlineStr">
+        <is>
+          <t>U/l</t>
+        </is>
+      </c>
+      <c r="L69" t="inlineStr">
+        <is>
+          <t>1.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="I70" t="inlineStr">
+        <is>
+          <t>ALT</t>
+        </is>
+      </c>
+      <c r="J70" t="inlineStr">
+        <is>
+          <t>56.33</t>
+        </is>
+      </c>
+      <c r="K70" t="inlineStr">
+        <is>
+          <t>U/l</t>
+        </is>
+      </c>
+      <c r="L70" t="inlineStr">
+        <is>
+          <t>1.53</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="I71" t="inlineStr">
+        <is>
+          <t>Total Bilirubin</t>
+        </is>
+      </c>
+      <c r="J71" t="inlineStr">
+        <is>
+          <t>10.67</t>
+        </is>
+      </c>
+      <c r="K71" t="inlineStr">
+        <is>
+          <t>mg/dl</t>
+        </is>
+      </c>
+      <c r="L71" t="inlineStr">
+        <is>
+          <t>4.72 *</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="I72" t="inlineStr">
+        <is>
+          <t>AST</t>
+        </is>
+      </c>
+      <c r="J72" t="inlineStr">
+        <is>
+          <t>122.33</t>
+        </is>
+      </c>
+      <c r="K72" t="inlineStr">
+        <is>
+          <t>U/l</t>
+        </is>
+      </c>
+      <c r="L72" t="inlineStr">
+        <is>
+          <t>2.52</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="I73" t="inlineStr">
+        <is>
+          <t>ALT</t>
+        </is>
+      </c>
+      <c r="J73" t="inlineStr">
+        <is>
+          <t>160.33</t>
+        </is>
+      </c>
+      <c r="K73" t="inlineStr">
+        <is>
+          <t>U/l</t>
+        </is>
+      </c>
+      <c r="L73" t="inlineStr">
+        <is>
+          <t>25.66 *</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="I74" t="inlineStr">
+        <is>
+          <t>Total Bilirubin</t>
+        </is>
+      </c>
+      <c r="J74" t="inlineStr">
+        <is>
+          <t>14.33</t>
+        </is>
+      </c>
+      <c r="K74" t="inlineStr">
+        <is>
+          <t>mg/dl</t>
+        </is>
+      </c>
+      <c r="L74" t="inlineStr">
+        <is>
+          <t>4.04 *</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="I75" t="inlineStr">
+        <is>
+          <t>AST</t>
+        </is>
+      </c>
+      <c r="J75" t="inlineStr">
+        <is>
+          <t>170.67</t>
+        </is>
+      </c>
+      <c r="K75" t="inlineStr">
+        <is>
+          <t>U/l</t>
+        </is>
+      </c>
+      <c r="L75" t="inlineStr">
+        <is>
+          <t>1.53</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="I76" t="inlineStr">
+        <is>
+          <t>ALT</t>
+        </is>
+      </c>
+      <c r="J76" t="inlineStr">
+        <is>
+          <t>146.33</t>
+        </is>
+      </c>
+      <c r="K76" t="inlineStr">
+        <is>
+          <t>U/l</t>
+        </is>
+      </c>
+      <c r="L76" t="inlineStr">
+        <is>
+          <t>32.52 *</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:K11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>Animal Model</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>Sample Size</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>Treatment 1</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>Dose 1</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
+          <t>Units 1</t>
+        </is>
+      </c>
+      <c r="F1" s="2" t="inlineStr">
+        <is>
+          <t>Treatment 2</t>
+        </is>
+      </c>
+      <c r="G1" s="2" t="inlineStr">
+        <is>
+          <t>Dose 2</t>
+        </is>
+      </c>
+      <c r="H1" s="2" t="inlineStr">
+        <is>
+          <t>Units 2</t>
+        </is>
+      </c>
+      <c r="I1" s="2" t="inlineStr">
+        <is>
+          <t>Biomarker</t>
+        </is>
+      </c>
+      <c r="J1" s="2" t="inlineStr">
+        <is>
+          <t>Frequency</t>
+        </is>
+      </c>
+      <c r="K1" s="2" t="inlineStr">
+        <is>
+          <t>Severity</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>Mortality rate</t>
+        </is>
+      </c>
+      <c r="J2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>methotrexate</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>0.2</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>mg/kg</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>Mortality rate</t>
+        </is>
+      </c>
+      <c r="J3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>aspartame</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>40</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>mg/kg</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>Mortality rate</t>
+        </is>
+      </c>
+      <c r="J4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>Mortality rate</t>
+        </is>
+      </c>
+      <c r="J5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>Mortality rate</t>
+        </is>
+      </c>
+      <c r="J6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>Mortality rate</t>
+        </is>
+      </c>
+      <c r="J7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>Mortality rate</t>
+        </is>
+      </c>
+      <c r="J8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>Mortality rate</t>
+        </is>
+      </c>
+      <c r="J9" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>Mortality rate</t>
+        </is>
+      </c>
+      <c r="J10" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>Mortality rate</t>
+        </is>
+      </c>
+      <c r="J11" t="n">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>